<commit_message>
- changed the sricpts used for running the training and trained the models on Python and C files - updated requirements.txt
</commit_message>
<xml_diff>
--- a/backend/HDHGN/work_dir/results_python.xlsx
+++ b/backend/HDHGN/work_dir/results_python.xlsx
@@ -450,14 +450,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 37 </t>
+          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 38 </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9324324324324325</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8918918918918919</v>
+        <v>0.4078947368421053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>